<commit_message>
Practical 1.1 & 1.2
</commit_message>
<xml_diff>
--- a/Analysis_Sheet.xlsx
+++ b/Analysis_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\0Programs\DAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F330E62-3D3D-42EE-B9B4-D0C275E6F863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016F6B46-6AAD-4C19-AD87-6849475CC250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{805A02CB-912E-462F-9CBC-A43655F66DFF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Iterative</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Factorial</t>
+  </si>
+  <si>
+    <t>Fibonnaci</t>
   </si>
 </sst>
 </file>
@@ -110,18 +113,18 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -990,6 +993,790 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Iterative</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.2'!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1.2'!$E$6:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.2'!$F$6:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-17D9-4DAE-B26A-375504BA31A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="1200257711"/>
+        <c:axId val="1200258191"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1200257711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200258191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1200258191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1200257711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Recursive</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.2'!$P$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1.2'!$O$6:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.2'!$P$6:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>292</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCC7-49EF-B5C3-41B2E4BA5A1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="1193562767"/>
+        <c:axId val="1193571887"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1193562767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1193571887"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1193571887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1193562767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1070,6 +1857,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
@@ -1609,6 +2476,1082 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2203,6 +4146,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EEF6150-0293-CF82-E7E3-065422281E83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A8E312-5998-D93F-5A3C-8058DA09D051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765F51D0-6388-7AAB-460C-602A1BC3D2EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2555,34 +4575,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
@@ -2601,16 +4621,16 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="4:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2769,8 +4789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E79700-AA80-45BF-9EEC-F65707456C2D}">
   <dimension ref="D1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2780,37 +4800,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="4:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="5"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2821,23 +4841,23 @@
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="4:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="5"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2846,13 +4866,13 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.3">
@@ -2860,7 +4880,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -2874,13 +4894,13 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O8">
         <v>3</v>
       </c>
       <c r="P8">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.3">
@@ -2888,13 +4908,13 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="O9">
         <v>4</v>
       </c>
       <c r="P9">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.3">
@@ -2902,13 +4922,13 @@
         <v>5</v>
       </c>
       <c r="F10">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="O10">
         <v>5</v>
       </c>
       <c r="P10">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.3">
@@ -2916,13 +4936,13 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="O11">
         <v>6</v>
       </c>
       <c r="P11">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.3">
@@ -2930,13 +4950,13 @@
         <v>7</v>
       </c>
       <c r="F12">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="O12">
         <v>7</v>
       </c>
       <c r="P12">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.3">
@@ -2944,13 +4964,13 @@
         <v>8</v>
       </c>
       <c r="F13">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="O13">
         <v>8</v>
       </c>
       <c r="P13">
-        <v>8</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.3">
@@ -2958,13 +4978,13 @@
         <v>9</v>
       </c>
       <c r="F14">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="O14">
         <v>9</v>
       </c>
       <c r="P14">
-        <v>9</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.3">
@@ -2972,13 +4992,13 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="O15">
         <v>10</v>
       </c>
       <c r="P15">
-        <v>10</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2988,5 +5008,6 @@
     <mergeCell ref="O3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Equations for every graph
</commit_message>
<xml_diff>
--- a/Analysis_Sheet.xlsx
+++ b/Analysis_Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\0Programs\DAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Programs\DAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016F6B46-6AAD-4C19-AD87-6849475CC250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627F121-15CC-48D1-81EB-63169CEF93E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{805A02CB-912E-462F-9CBC-A43655F66DFF}"/>
   </bookViews>
@@ -309,6 +309,55 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.39194217172364854"/>
+                  <c:y val="0.21087489063867015"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'1.1'!$D$6:$D$15</c:f>
@@ -730,6 +779,55 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.33578817353713136"/>
+                  <c:y val="0.1571168708078157"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'1.1'!$N$6:$N$15</c:f>
@@ -1151,6 +1249,55 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.36103193350831148"/>
+                  <c:y val="0.13262284922717993"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'1.2'!$E$6:$E$15</c:f>
@@ -1515,6 +1662,49 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'1.2'!$O$6:$O$15</c:f>
@@ -4562,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51522124-DBA8-4FFF-993E-D9D3F30E332D}">
   <dimension ref="D1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4790,7 +4980,7 @@
   <dimension ref="D1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Equations in Graphs
</commit_message>
<xml_diff>
--- a/Analysis_Sheet.xlsx
+++ b/Analysis_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Programs\DAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627F121-15CC-48D1-81EB-63169CEF93E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FEE02A-D723-4771-AAAD-687FDF69EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{805A02CB-912E-462F-9CBC-A43655F66DFF}"/>
   </bookViews>
@@ -4979,7 +4979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E79700-AA80-45BF-9EEC-F65707456C2D}">
   <dimension ref="D1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>

</xml_diff>